<commit_message>
update files and insert times into dat file
</commit_message>
<xml_diff>
--- a/ModelingV0/output/data/instance_9_betamaior.xlsx
+++ b/ModelingV0/output/data/instance_9_betamaior.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,6 +570,831 @@
       <c r="G4" t="inlineStr">
         <is>
           <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['00000001_F3']</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['UE4']</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>['F3', 'SBS4', 'MBS2', 'SBS5', 'UE4']</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['UE3']</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'SBS5', 'UE3']</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['00000003_F3']</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>['UE1']</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>['F3', 'SBS4', 'MBS2', 'MBS1', 'SBS1', 'UE1']</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['00000001_F3']</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>['UE4']</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>['F3', 'SBS4', 'MBS2', 'SBS5', 'UE4']</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>['UE3']</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'MBS1', 'SBS1', 'UE3']</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['00000003_F3']</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>['UE1']</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>['F3', 'SBS4', 'MBS2', 'MBS1', 'SBS1', 'UE1']</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>['UE2']</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'SBS4', 'UE2']</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['00000001_F3']</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>['UE4']</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>['F3', 'SBS4', 'MBS2', 'SBS5', 'UE4']</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>['UE3']</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'MBS1', 'SBS1', 'UE3']</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>['00000003_F3']</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>['UE1']</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>['F3', 'SBS4', 'MBS2', 'MBS1', 'SBS1', 'UE1']</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>['UE2']</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'MBS1', 'SBS2', 'UE2']</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>['00000005_F1']</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>['UE4']</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'SBS5', 'UE4']</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>['00000001_F3']</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>['UE4']</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>['F3', 'SBS4', 'MBS2', 'SBS5', 'UE4']</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>['UE3']</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'MBS1', 'SBS1', 'UE3']</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>['00000003_F3']</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>['UE1']</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>['F3', 'SBS4', 'MBS2', 'MBS1', 'SBS1', 'UE1']</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>['UE2']</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'MBS1', 'SBS3', 'UE2']</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>['00000005_F1']</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['UE4']</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'SBS5', 'UE4']</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>['00000006_F2']</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>['F2']</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>['UE1']</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>['F2', 'SBS4', 'UE1']</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>['00000001_F3']</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>['UE4']</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>['F3', 'SBS4', 'MBS2', 'SBS5', 'UE4']</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>['UE3']</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'SBS4', 'UE3']</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>['00000003_F3']</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>['UE1']</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>['F3', 'SBS4', 'MBS2', 'MBS1', 'SBS1', 'UE1']</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>['UE2']</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'MBS1', 'SBS1', 'UE2']</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>['00000005_F1']</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>['UE4']</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>['F1', 'MBS2', 'SBS5', 'UE4']</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>MBS2</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>['00000006_F2']</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>['F2']</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>['UE1']</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>['F2', 'SBS4', 'MBS2', 'MBS1', 'SBS1', 'UE1']</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>SBS4</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>['00000007_F2']</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>['F2']</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>['UE2']</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>['F2', 'SBS4', 'MBS2', 'MBS1', 'SBS1', 'UE2']</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>SBS4</t>
         </is>
       </c>
     </row>
@@ -710,10 +1535,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2857142857142857</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D2" t="n">
         <v>7</v>
@@ -976,7 +1801,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1040,7 +1865,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20">
@@ -1104,7 +1929,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1168,7 +1993,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="28">
@@ -1232,7 +2057,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1387,7 +2212,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1453,7 +2278,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE3')</t>
+          <t>('SBS4', 'MBS2')</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1465,11 +2290,11 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE4')</t>
+          <t>('MBS1', 'SBS1')</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1481,11 +2306,11 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>('SBS4', 'MBS2')</t>
+          <t>('MBS2', 'MBS1')</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1497,15 +2322,15 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>('F1', 'MBS2')</t>
+          <t>('MBS2', 'SBS5')</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
@@ -1513,15 +2338,15 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>('F3', 'SBS4')</t>
+          <t>('SBS4', 'MBS2')</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9">
@@ -1529,7 +2354,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1545,7 +2370,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1561,11 +2386,11 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE3')</t>
+          <t>('MBS2', 'SBS4')</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -1577,11 +2402,11 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE4')</t>
+          <t>('MBS2', 'SBS5')</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1593,7 +2418,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1601,7 +2426,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14">
@@ -1609,15 +2434,15 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>('F1', 'MBS2')</t>
+          <t>('MBS1', 'SBS1')</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>45</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15">
@@ -1625,15 +2450,15 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>('F3', 'SBS4')</t>
+          <t>('MBS2', 'MBS1')</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>45</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16">
@@ -1641,15 +2466,15 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>('MBS1', 'SBS1')</t>
+          <t>('MBS2', 'SBS4')</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17">
@@ -1657,11 +2482,11 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>('MBS2', 'MBS1')</t>
+          <t>('MBS2', 'SBS5')</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1673,191 +2498,15 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE3')</t>
+          <t>('SBS4', 'MBS2')</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>3</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>('SBS1', 'UE4')</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>3</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>('SBS4', 'MBS2')</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>3</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>('F1', 'MBS2')</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>3</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>('F3', 'SBS4')</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>4</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>('MBS1', 'SBS1')</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>4</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>('MBS2', 'MBS1')</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>4</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>('SBS1', 'UE3')</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>4</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>('SBS1', 'UE4')</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>4</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>('SBS4', 'MBS2')</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="n">
-        <v>4</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>('F1', 'MBS2')</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="n">
-        <v>4</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>('F3', 'SBS4')</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>45</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1871,7 +2520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1981,11 +2630,11 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>('F1', 'MBS2')</t>
+          <t>('MBS1', 'SBS1')</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -1997,11 +2646,11 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>('F3', 'SBS4')</t>
+          <t>('MBS2', 'MBS1')</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -2017,7 +2666,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>('MBS1', 'SBS1')</t>
+          <t>('MBS2', 'SBS5')</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -2033,11 +2682,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>('MBS2', 'MBS1')</t>
+          <t>('SBS1', 'UE1')</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
@@ -2049,11 +2698,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE3')</t>
+          <t>('SBS4', 'MBS2')</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12">
@@ -2065,7 +2714,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE4')</t>
+          <t>('SBS5', 'UE3')</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -2081,7 +2730,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>('SBS4', 'MBS2')</t>
+          <t>('SBS5', 'UE4')</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -2093,15 +2742,15 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>('F1', 'MBS2')</t>
+          <t>('MBS1', 'SBS1')</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
@@ -2109,15 +2758,15 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>('F3', 'SBS4')</t>
+          <t>('MBS2', 'MBS1')</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16">
@@ -2129,11 +2778,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>('MBS1', 'SBS1')</t>
+          <t>('MBS2', 'SBS4')</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17">
@@ -2145,11 +2794,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>('MBS2', 'MBS1')</t>
+          <t>('MBS2', 'SBS5')</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18">
@@ -2161,7 +2810,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE3')</t>
+          <t>('SBS1', 'UE1')</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -2177,7 +2826,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE4')</t>
+          <t>('SBS1', 'UE3')</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -2197,7 +2846,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21">
@@ -2209,7 +2858,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>('F1', 'MBS2')</t>
+          <t>('SBS4', 'UE2')</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -2225,7 +2874,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>('F3', 'SBS4')</t>
+          <t>('SBS5', 'UE4')</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -2245,7 +2894,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24">
@@ -2261,7 +2910,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25">
@@ -2273,7 +2922,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE3')</t>
+          <t>('MBS2', 'SBS4')</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2289,11 +2938,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>('SBS1', 'UE4')</t>
+          <t>('MBS2', 'SBS5')</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27">
@@ -2305,11 +2954,11 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>('SBS4', 'MBS2')</t>
+          <t>('SBS1', 'UE1')</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28">
@@ -2321,11 +2970,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>('F1', 'MBS2')</t>
+          <t>('SBS1', 'UE2')</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29">
@@ -2337,11 +2986,43 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>('F3', 'SBS4')</t>
+          <t>('SBS4', 'MBS2')</t>
         </is>
       </c>
       <c r="D29" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>('SBS4', 'UE3')</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
         <v>45</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>('SBS5', 'UE4')</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2355,7 +3036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2391,25 +3072,388 @@
       <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['00000001_F3']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['00000003_F3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['00000001_F3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['00000003_F3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['00000001_F3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>['00000003_F3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>['00000005_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>['00000001_F3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>['00000005_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>['00000003_F3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>['00000005_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>['00000001_F3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>['00000005_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>['00000002_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>['00000004_F1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>['00000006_F2']</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>